<commit_message>
Continuacao do projeto fluxo de caixa
</commit_message>
<xml_diff>
--- a/Excel/secao_14_projeto_final/projeto_fluxo_de_caixa.xlsx
+++ b/Excel/secao_14_projeto_final/projeto_fluxo_de_caixa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.gomes\Desktop\Cursos\Excel\secao_14_projeto_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC519DA0-7F87-4DAE-930F-CA2B4DC9C61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44225A94-1964-4049-AE32-53F6FF5478FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{B0F91605-3ADC-4A73-9DEB-952AC89617AD}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="6" xr2:uid="{B0F91605-3ADC-4A73-9DEB-952AC89617AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,12 @@
     <sheet name="DashBoardFinanceiroAtual" sheetId="15" r:id="rId15"/>
     <sheet name="DashBoardFinanceiroMensal" sheetId="16" r:id="rId16"/>
   </sheets>
+  <definedNames>
+    <definedName name="PCEntradasN1_Nivel_1">TbPcEntradasN1[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nivel_1">TbPCEntradasN2[[Nível 1 ]]</definedName>
+    <definedName name="PCEntradasN2_Nivel_2">TbPCEntradasN2[Nível 2]</definedName>
+    <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -109,12 +115,156 @@
   </si>
   <si>
     <t>DASHBOARD FINANCEIRO MENSAL</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE ENTRADA NÍVEL 1</t>
+  </si>
+  <si>
+    <t>Nível 1</t>
+  </si>
+  <si>
+    <t>Empréstimos de curto prazo</t>
+  </si>
+  <si>
+    <t>Financiamentos de longo prazo</t>
+  </si>
+  <si>
+    <t>Receitas Financeiras</t>
+  </si>
+  <si>
+    <t>Venda de ativos</t>
+  </si>
+  <si>
+    <t>Vendas de mercadorias</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE ENTRADAS NÍVEL 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nível 1 </t>
+  </si>
+  <si>
+    <t>Nível 2</t>
+  </si>
+  <si>
+    <t>Empréstimo de curto prazo</t>
+  </si>
+  <si>
+    <t>Empréstimos capital de giro</t>
+  </si>
+  <si>
+    <t>Juros sobre aplicações</t>
+  </si>
+  <si>
+    <t>Mobiliário próprio</t>
+  </si>
+  <si>
+    <t>Eletrodomésticos</t>
+  </si>
+  <si>
+    <t>Informática</t>
+  </si>
+  <si>
+    <t>Livros</t>
+  </si>
+  <si>
+    <t>Móveis</t>
+  </si>
+  <si>
+    <t>Som e imagem</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE SAÍDA NÍVEL 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compra de mercadorias</t>
+  </si>
+  <si>
+    <t>Despesas administrativas</t>
+  </si>
+  <si>
+    <t>Despesas comerciais</t>
+  </si>
+  <si>
+    <t>Despesas financeiras</t>
+  </si>
+  <si>
+    <t>Imposto de renda</t>
+  </si>
+  <si>
+    <t>Imposto sobre as vendas</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE SAÍDA NÍVEL 2</t>
+  </si>
+  <si>
+    <t>Som e Imagem</t>
+  </si>
+  <si>
+    <t>Vestuário</t>
+  </si>
+  <si>
+    <t>Comunicação - internet e telefonia</t>
+  </si>
+  <si>
+    <t>Energia elétrica</t>
+  </si>
+  <si>
+    <t>Encargos sobre os salários dos vendedores</t>
+  </si>
+  <si>
+    <t>Salários dos vendedores</t>
+  </si>
+  <si>
+    <t>Juros sobre empréstimos</t>
+  </si>
+  <si>
+    <t>IR sobre o lucro presumido</t>
+  </si>
+  <si>
+    <t>Data do Caixa Realizado</t>
+  </si>
+  <si>
+    <t>Data da competência</t>
+  </si>
+  <si>
+    <t>Data do Caixa Previsto</t>
+  </si>
+  <si>
+    <t>Conta Nível 1</t>
+  </si>
+  <si>
+    <t>Conta Nível 2</t>
+  </si>
+  <si>
+    <t>Hostórico</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>NF001</t>
+  </si>
+  <si>
+    <t>NF773</t>
+  </si>
+  <si>
+    <t>NF2639</t>
+  </si>
+  <si>
+    <t>NF-16</t>
+  </si>
+  <si>
+    <t>Geral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,7 +327,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,8 +352,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,11 +367,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -224,28 +421,145 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="2" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="2" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color theme="2" tint="-0.24994659260841701"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2962,6 +3276,64 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6036148-4E03-4169-B923-183719B8F8F1}" name="TbPcEntradasN1" displayName="TbPcEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="B4:B9" xr:uid="{F6036148-4E03-4169-B923-183719B8F8F1}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8497777F-EEC2-4246-9694-C79DD6F062C6}" name="Nível 1" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4B1F385-4C25-4C7F-9D90-AE28445CED30}" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B4:C13" xr:uid="{A4B1F385-4C25-4C7F-9D90-AE28445CED30}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{43418F28-3016-432A-9CB8-B75F2638B401}" name="Nível 1 "/>
+    <tableColumn id="2" xr3:uid="{B498796E-8180-4B47-936D-A2B700172D98}" name="Nível 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3DF6199E-B54F-469A-BF78-DB03614FDD1B}" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="B4:B10" xr:uid="{3DF6199E-B54F-469A-BF78-DB03614FDD1B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{C8164EAC-3156-4EB9-8E8F-2FC26A396EB4}" name="Nível 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6AA1FA7F-9F0B-4046-BF4A-BCBD800ADA22}" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B4:C15" xr:uid="{6AA1FA7F-9F0B-4046-BF4A-BCBD800ADA22}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{217D2477-5E6B-41F4-9F0A-9C0266BD4A7A}" name="Nível 1"/>
+    <tableColumn id="2" xr3:uid="{A6E0B336-1F05-450F-A33A-A99A02491CF2}" name="Nível 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{77800E36-C2B8-4EC2-BA85-D563A774B892}" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="B3:H7" xr:uid="{77800E36-C2B8-4EC2-BA85-D563A774B892}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{4C1805C6-7AD3-4723-B94B-809B50706F76}" name="Data do Caixa Realizado" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{E84FFBC0-A48C-4D30-8C19-E752EEA9620D}" name="Data da competência" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{7A123657-EF7A-4BCD-8BD2-753F722131B0}" name="Data do Caixa Previsto" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D9314CB5-B4C5-4D33-AA25-0655FBD86A86}" name="Conta Nível 1"/>
+    <tableColumn id="5" xr3:uid="{3552428F-2F1E-445E-9663-B6E33FD08B49}" name="Conta Nível 2"/>
+    <tableColumn id="6" xr3:uid="{DA56175D-677F-431C-9BD4-1185027168F4}" name="Hostórico"/>
+    <tableColumn id="7" xr3:uid="{A52F080A-E3C3-4B04-BB75-8AF1187ABB56}" name="Valor" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3266,7 +3638,7 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3287,14 +3659,14 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3355,10 +3727,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3380,34 +3752,46 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I5" s="5"/>
     </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>
@@ -3449,29 +3833,29 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -3493,10 +3877,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,34 +3902,46 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I5" s="5"/>
     </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>
@@ -3562,214 +3958,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I5" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B2:N2"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1899D21F-7BAD-4069-AFB6-518F9D80C6AA}">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I5" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B2:N2"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE70B4D-8C0A-4897-90E1-143CE5AD9BCA}">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I5" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B2:N2"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072786B8-D1DC-40EA-8FCA-2E021835854E}">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
@@ -3794,34 +3983,289 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="I1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I5" s="5"/>
     </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="B2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1899D21F-7BAD-4069-AFB6-518F9D80C6AA}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="B2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE70B4D-8C0A-4897-90E1-143CE5AD9BCA}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="B2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072786B8-D1DC-40EA-8FCA-2E021835854E}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>
@@ -3863,29 +4307,29 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -3907,10 +4351,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3932,34 +4377,102 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+    </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="5"/>
     </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>
@@ -3968,6 +4481,9 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3976,10 +4492,199 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G1:N1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B13" xr:uid="{2862B469-29CF-4B0E-A240-7DDA7FDEC5E8}">
+      <formula1>PCEntradasN1_Nivel_1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B5:C5" listDataValidation="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB400DB-58B3-49A9-9A09-4D78B0DC91FE}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,34 +4706,95 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="I1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
       <c r="I5" s="5"/>
     </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>
@@ -4037,18 +4803,401 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB400DB-58B3-49A9-9A09-4D78B0DC91FE}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A27515-8031-4110-8822-D749CD9C0760}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F1:N1"/>
+  </mergeCells>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B15" xr:uid="{8C76D652-69E9-463C-9C21-ABA019112F45}">
+      <formula1>PCSaídasN1_Nível_1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C105092-CBD4-4073-B9F9-D933203CB72F}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="57" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="2:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="25">
+        <v>43146</v>
+      </c>
+      <c r="C4" s="25">
+        <v>43146</v>
+      </c>
+      <c r="D4" s="25">
+        <v>43146</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="25">
+        <v>43530</v>
+      </c>
+      <c r="C5" s="25">
+        <v>43466</v>
+      </c>
+      <c r="D5" s="25">
+        <v>43496</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="26">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="25">
+        <v>43467</v>
+      </c>
+      <c r="C6" s="25">
+        <v>43467</v>
+      </c>
+      <c r="D6" s="25">
+        <v>43467</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="26">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="25">
+        <v>43535</v>
+      </c>
+      <c r="C7" s="25">
+        <v>43467</v>
+      </c>
+      <c r="D7" s="25">
+        <v>43497</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7" xr:uid="{75F523B8-8FFC-495F-AB1C-A4320280E97F}">
+      <formula1>PCEntradasN1_Nivel_1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7" xr:uid="{C95E0B48-100E-4A09-8C7C-211C1CC12388}">
+      <formula1>OFFSET(PCEntradasN2_Nivel_2,MATCH(E4,PCEntradasN2_Nivel_1,0)-1,0,COUNTIF(PCEntradasN2_Nivel_1,E4)-0)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8445458-0364-44E7-9830-197173E0980D}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4070,239 +5219,46 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="I1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I5" s="5"/>
     </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B2:N2"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A27515-8031-4110-8822-D749CD9C0760}">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I5" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B2:N2"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C105092-CBD4-4073-B9F9-D933203CB72F}">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I5" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B2:N2"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8445458-0364-44E7-9830-197173E0980D}">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I5" s="5"/>
-    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>
@@ -4319,7 +5275,7 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -4344,37 +5300,49 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="2:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="C6" s="10"/>
-    </row>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>

</xml_diff>